<commit_message>
minor tweaks and formatting
</commit_message>
<xml_diff>
--- a/my_music_history.xlsx
+++ b/my_music_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D361"/>
+  <dimension ref="A1:D362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6562,6 +6562,26 @@
         </is>
       </c>
     </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Adele</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
integrate latest gkeep data into working
data is fetched from gkeep account after every run
added function to update previous spotify logs when 'arrow' moves ahead
</commit_message>
<xml_diff>
--- a/my_music_history.xlsx
+++ b/my_music_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F362"/>
+  <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LONG.LIVE.A$AP (Deluxe Version)</t>
+          <t>LONG.LIVE.A$AP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kanye West</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['2017', 'hip-hop', 'east coast hip-hop', 'political', 'rap']</t>
+          <t>['hip-hop', '2017', 'rap', 'east coast hip hop', 'conscious hip hop']</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['rap', 'lil wayne', 'hip-hop', '2008', 'hip hop']</t>
+          <t>['rap', 'lil wayne', 'hip-hop', '2008', 'best of 2008']</t>
         </is>
       </c>
     </row>
@@ -882,14 +882,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>J. Cole</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2014 Forest Hills Drive (Live)</t>
+          <t>2014 Forest Hills Drive (LIVE)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -899,17 +895,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['hip-hop', 'rap', 'j cole', 'hip hop', 'north carolina']</t>
+          <t>['Error fetch']</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1065,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', '2018', 'hip hop', 'trap']</t>
+          <t>['rap', 'hip-hop', 'hip hop', '2018', 'trap']</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1129,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['chicago', '2018', 'jazz rap', 'rap', 'hip-hop']</t>
+          <t>['chicago', 'rap', 'hip-hop', 'jazz rap', 'conscious hip hop']</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1151,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>22 tracks, 74:35</t>
+          <t>22 tracks, 74:36</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1219,7 +1215,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14 tracks, 53:44</t>
+          <t>14 tracks, 54:02</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1325,14 +1321,14 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['2018', 'trap', 'trap metal', 'hip-hop', 'cloud rap']</t>
+          <t>['2018', 'trap', 'trap metal', 'hip-hop', 'rap']</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Denzel Curry</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1357,7 +1353,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', 'denzel curry', 'trap', 'furry']</t>
+          <t>['rap', 'denzel curry', 'hip-hop', 'trap', 'furry']</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1513,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['rap', 'kid cudi', 'kanye west', 'hip-hop', 'pop rap']</t>
+          <t>['rap', 'kid cudi', 'kanye west', 'hip-hop', 'art pop']</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1525,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Man on the Moon: The End of Day</t>
+          <t>Man On The Moon: The End Of Day</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1539,29 +1535,25 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15 tracks</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1 January 2009</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['hip-hop', 'kid cudi', 'rap', 'hip hop', 'chill']</t>
+          <t>['hip hop', 'synthpop', 'neo-psychedelia', 'art pop', 'pop rap']</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Kid Cudi</t>
-        </is>
-      </c>
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Man on the Moon II: The Legend of Mr. Rager</t>
+          <t>Man On The Moon 2: The Legend Of Rager</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1571,17 +1563,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>17 tracks</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1 January 2010</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['hip-hop', 'alternative', 'rap', 'kid cudi', 'alternative rap']</t>
+          <t>['Error fetch']</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1809,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Free 6LACK</t>
+          <t>FREE 6LACK</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1827,17 +1819,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14 tracks</t>
+          <t>15 tracks</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>14 tracks</t>
+          <t>13 November 2017</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['trap', 'alternative rnb', 'rnb', 'hip-hop', '2016']</t>
+          <t>['6lack', 'rnb', 'rap', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -1933,7 +1925,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['trap', 'emo rap', '2017', 'hip-hop', 'lil uzi vert']</t>
+          <t>['trap', 'emo rap', 'hip-hop', '2017', 'lil uzi vert']</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2117,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['hip-hop', 'rap', 'kanye west', 'hip hop', 'rnb']</t>
+          <t>['hip-hop', 'rap', 'kanye west', 'hip hop', 'soul']</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2245,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', 'trap', 'pop rap', 'hip hop']</t>
+          <t>['rap', 'hip-hop', 'trap', 'hip hop', 'pop rap']</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2277,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>['alternative', 'saw live', 'my music library', 'rnb', 'australian']</t>
+          <t>['alternative', 'saw live', 'rnb', 'peak', 'chase atlantic']</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2309,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>['rnb', 'hip hop', 'trap', 'hip-hop', 'alternative rnb']</t>
+          <t>['rnb', 'alternative rnb', 'trap', 'rap', 'hip hop']</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2373,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['rap', 'hip hop', 'jazz rap', 'neo-soul', 'pop rap']</t>
+          <t>['rap', 'jazz rap', 'hip hop', 'neo-soul', 'pop rap']</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2405,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>['hip-hop', 'rap', 'hip hop', 'male vocalists', 'experimental hip-hop']</t>
+          <t>['hip-hop', 'rap', 'hip hop', 'male vocalists', 'trap rap']</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2437,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>['rap', 'hardcore hip hop', 'experimental hip hop', 'hip-hop', 'hip hop']</t>
+          <t>['hardcore hip hop', 'rap', 'experimental hip hop', 'hip-hop', 'hip hop']</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2469,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>['indie rock', 'americana', 'folk rock', 'roots rock', 'folk']</t>
+          <t>['indie rock', 'americana', 'folk rock', 'folk', 'roots rock']</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2693,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>['rap', 'pop rap', 'hip-hop', '2013', 'west coast hip hop']</t>
+          <t>['rap', 'pop rap', 'hip-hop', 'west coast hip hop', '2013']</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2725,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>['2013', 'hip hop', 'rap', 'hip-hop', 'chance the rapper']</t>
+          <t>['rap', '2013', 'hip-hop', 'chance the rapper', 'pop rap']</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2789,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>['rap', 'gangsta rap', 'drill', 'banger', 'hip-hop']</t>
+          <t>['rap', 'gangsta rap', 'drill', 'banger', 'chief keef']</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2821,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>['rnb', 'lana del rey', 'canadian', 'dance', 'synthpop']</t>
+          <t>['rnb', 'lana del rey', 'canadian', 'dance', 'pop']</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2885,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>['southern hip hop', 'neo-soul', 'rap', 'hip-hop', 'hip hop']</t>
+          <t>['southern hip hop', 'neo-soul', 'rap', 'hip-hop', 'southern hip-hop']</t>
         </is>
       </c>
     </row>
@@ -2925,7 +2917,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>['cringe', 'hip-hop', 'trap', 'hardcore hip-hop', '2018']</t>
+          <t>['rap', 'boom bap', '2018', 'cringe', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2949,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>['nipsey hussle', 'hip-hop', 'rap', 'west coast rap', 'gangsta rap']</t>
+          <t>['nipsey hussle', 'hip-hop', 'rap', 'gangsta rap', 'west coast rap']</t>
         </is>
       </c>
     </row>
@@ -2989,7 +2981,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>['hip-hop', 'emo rap', 'emo', 'rap', 'cloud rap']</t>
+          <t>['emo', 'hip-hop', 'rap', 'emo rap', 'cloud rap']</t>
         </is>
       </c>
     </row>
@@ -3075,7 +3067,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13 tracks, 48:11</t>
+          <t>13 tracks, 51:35</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3129,7 +3121,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>uknowhatimsayinÂ¿</t>
+          <t>uknowhatimsayinÃ‚Â¿</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3289,7 +3281,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>King Push â€“ Darkest Before Dawn: The Prelude</t>
+          <t>King Push - Darkest Before Dawn: The Prelude</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3395,7 +3387,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>13 tracks, 35:14</t>
+          <t>13 tracks, 35:16</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3405,14 +3397,14 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>['rap', 'trap', '21st century in music', 'hip-hop', 'hip hop']</t>
+          <t>['rap', 'trap', '2019', '21st century in music', 'hip-hop']</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>DaBaby</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3437,7 +3429,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>['2019', 'hip-hop', 'dababy', '7', '2010s']</t>
+          <t>['dababy', '2019', '21st century in music', 'hip-hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -3636,7 +3628,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>$ilkMoney</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3796,7 +3788,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Matmos</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3924,7 +3916,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Beast Coast</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3956,7 +3948,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Freddie Gibbs</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -4020,7 +4012,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>$ilkMoney</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4084,7 +4076,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>BROCKHAMPTON</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -4148,29 +4140,29 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
+          <t>Roots</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>UNDUN</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
           <t>Error fetch</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>UNDUN</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
+      <c r="E117" t="inlineStr">
         <is>
           <t>Error fetch</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
       <c r="F117" t="inlineStr">
         <is>
           <t>['Error fetch']</t>
@@ -4178,11 +4170,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A118" t="inlineStr"/>
       <c r="B118" t="inlineStr">
         <is>
           <t>Stream Of Though Vol. 1</t>
@@ -4237,7 +4225,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', 'melodic rap', '2019', 'rap']</t>
+          <t>['rap', 'hip-hop', 'melodic rap', '2019', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -4306,11 +4294,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A122" t="inlineStr"/>
       <c r="B122" t="inlineStr">
         <is>
           <t>Replay Jassie Gill</t>
@@ -4340,7 +4324,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Denzel Curry</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -4493,7 +4477,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>['2020', 'rap', 'hip-hop', 'funk', 'childish gambino']</t>
+          <t>['2020', 'rap', 'hip-hop', 'funk', 'hip hop']</t>
         </is>
       </c>
     </row>
@@ -4525,7 +4509,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>['2024', 'pop', 'synthpop', 'alt-pop', 'pop']</t>
+          <t>['2024', 'pop', 'synthpop', 'alt-pop', 'vinyl wishlist']</t>
         </is>
       </c>
     </row>
@@ -4562,11 +4546,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A130" t="inlineStr"/>
       <c r="B130" t="inlineStr">
         <is>
           <t>I am &gt; I was</t>
@@ -4621,7 +4601,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>['neo-soul', 'psychedelic soul', 'experimental hip hop', 'alternative rnb', 'pop rap']</t>
+          <t>['neo-soul', 'psychedelic soul', 'experimental hip hop', 'alternative rnb', 'hardcore hip hop']</t>
         </is>
       </c>
     </row>
@@ -4653,7 +4633,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>['mozzaddy', 'glitch hop', 'cloud rap', 'experimental', 'hardcore hip hop']</t>
+          <t>['mozzaddy', 'glitch hop', 'cloud rap', 'hardcore hip hop', 'industrial hip hop']</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4655,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>14 tracks, 56:15</t>
+          <t>14 tracks, 56:16</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -4692,7 +4672,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Lil Uzi Vert</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4717,7 +4697,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>['2020', '7', 'rap', 'hip-hop', 'trap']</t>
+          <t>['2020', 'trap', '7', 'rap', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -4739,7 +4719,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>11 tracks, 40:34</t>
+          <t>11 tracks, 37:17</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -4756,7 +4736,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>clipping., La Chat</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4788,7 +4768,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>clipping.</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4813,7 +4793,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>['hip-hop', 'experimental hip-hop', 'noise', 'experimental', 'rap']</t>
+          <t>['hip-hop', 'experimental hip-hop', 'experimental', 'noise', 'rap']</t>
         </is>
       </c>
     </row>
@@ -4845,7 +4825,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>['hip-hop', 'kanye west', 'rap', 'hip hop', 'skit']</t>
+          <t>['hip-hop', 'rap', 'kanye west', 'hip hop', 'skit']</t>
         </is>
       </c>
     </row>
@@ -4877,7 +4857,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>['gothic rock', 'goth rock', 'british', 'goth', 'radio caprice - darkwave']</t>
+          <t>['gothic rock', 'goth rock', 'british', 'goth', 'gothic metal']</t>
         </is>
       </c>
     </row>
@@ -4980,7 +4960,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>Pink Siifu</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -5012,7 +4992,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>Lupe Fiasco</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -5076,7 +5056,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Tyler, the Creator</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -5261,7 +5241,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>['2011', 'folk', 'indie', 'best of 2011', 'indie folk']</t>
+          <t>['2011', 'folk', 'best of 2011', 'indie', 'indie folk']</t>
         </is>
       </c>
     </row>
@@ -5293,16 +5273,12 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>['rap', '2020', 'hip hop', 'hip-hop', 'pop']</t>
+          <t>['2020', 'rap', 'hip hop', 'hip-hop', 'pop']</t>
         </is>
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A153" t="inlineStr"/>
       <c r="B153" t="inlineStr">
         <is>
           <t>BLOOD IN + BLOOD OUT</t>
@@ -5362,11 +5338,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A155" t="inlineStr"/>
       <c r="B155" t="inlineStr">
         <is>
           <t>4:44</t>
@@ -5485,7 +5457,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>['blues', 'john mayer', 'rock', 'pop', 'singer-songwriter']</t>
+          <t>['singer-songwriter', 'blues', 'acoustic', 'john mayer', 'rock']</t>
         </is>
       </c>
     </row>
@@ -5603,7 +5575,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>15 tracks, 50:24</t>
+          <t>15 tracks, 50:54</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -5709,7 +5681,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>['electronic', 'disco', 'funk', '2013', 'house']</t>
+          <t>['electronic', 'disco', '2013', 'funk', 'house']</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5777,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>['rap', 'acoustic', 'aries', 'pop-punk', 'rnb']</t>
+          <t>['rnb', 'hip-hop', 'pop', 'rap', 'soul']</t>
         </is>
       </c>
     </row>
@@ -5827,7 +5799,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>16 tracks, 51:06</t>
+          <t>16 tracks, 51:24</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -5837,7 +5809,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>['horrorcore', '2020', 'industrial hip hop', 'experimental hip hop', 'witch house']</t>
+          <t>['horrorcore', 'industrial hip hop', '2020', 'witch house', 'experimental hip hop']</t>
         </is>
       </c>
     </row>
@@ -6420,7 +6392,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Wynne</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -6541,7 +6513,7 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>['southern hip hop', 'jazz rap', 'rap', '2016', 'conscious hip hop']</t>
+          <t>['2016', 'southern hip hop', 'jazz rap', 'rap', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -6573,7 +6545,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>['2018', 'vinyl', 'rap', 'hip hop', 'west coast hip-hop']</t>
+          <t>['2018', 'rap', 'vince staples', 'nrg_scrobbler', 'hip hop']</t>
         </is>
       </c>
     </row>
@@ -6605,7 +6577,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>['hyperpop', '2020', 'electronic', 'tok1d', 'punk']</t>
+          <t>['hyperpop', '2020', 'electronic', 'tok1d', 'rap']</t>
         </is>
       </c>
     </row>
@@ -6644,7 +6616,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>will hyde</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -6701,7 +6673,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>['west coast hip hop', 'hip-hop', 'hardcore hip hop', 'rap', 'experimental hip hop']</t>
+          <t>['west coast hip hop', 'hip-hop', 'hardcore hip hop', 'rap', 'bubblegum bass']</t>
         </is>
       </c>
     </row>
@@ -6861,7 +6833,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>['hip-hop', '2018', 'finished', 'rap', 'producer']</t>
+          <t>['hip-hop', 'rap', '2018', 'finished', 'producer']</t>
         </is>
       </c>
     </row>
@@ -6996,7 +6968,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Mavi (12)</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -7218,11 +7190,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A213" t="inlineStr"/>
       <c r="B213" t="inlineStr">
         <is>
           <t>Stream of Thought, Vol. 3: Cane &amp; Able</t>
@@ -7316,7 +7284,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>R.A.P Ferreira</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -7373,7 +7341,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>['hip-hop', 'doom', 'mf doom', 'abstract hiphop', 'underground hip-hop']</t>
+          <t>['hip-hop', 'doom', 'mf doom', 'underground hip-hop', 'abstract hiphop']</t>
         </is>
       </c>
     </row>
@@ -7533,16 +7501,12 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>['a artist', 'trap', 'pop', 'electronic', 'goodshit']</t>
+          <t>['trap', 'pop', 'a artist', 'my top songs', 'electronic']</t>
         </is>
       </c>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A223" t="inlineStr"/>
       <c r="B223" t="inlineStr">
         <is>
           <t>Heaven Or Hell</t>
@@ -7597,7 +7561,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>['hip-hop', 'east coast rap', 'underground hip hop', 'rap', 'east coast hip hop']</t>
+          <t>['hip-hop', 'rap', 'hip hop', 'boom bap', 'east coast rap']</t>
         </is>
       </c>
     </row>
@@ -7629,7 +7593,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>['2020', 'synthpop', 'rnb', 'lo-fi', 'alternative rnb']</t>
+          <t>['alternative rnb', 'synthpop', 'personal favourites', 'alt-pop', 'pop rap']</t>
         </is>
       </c>
     </row>
@@ -7725,7 +7689,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>['trap', 'snot', 'chill', 'rap', 'lo-fi']</t>
+          <t>['trap', 'snot', 'chill', 'rap', 'hip-hop']</t>
         </is>
       </c>
     </row>
@@ -7821,7 +7785,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>['slow jam', 'rap', 'hip-hop', 'hip hop', '2019']</t>
+          <t>['slow jam', 'rap', 'hip-hop', 'hip hop', 'danceable']</t>
         </is>
       </c>
     </row>
@@ -7853,7 +7817,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>['hip hop', '2014', 'hip-hop', 'southern hip hop', 'tennessee']</t>
+          <t>['2014', 'hip hop', 'southern hip hop', 'hip-hop', 'rap']</t>
         </is>
       </c>
     </row>
@@ -7988,7 +7952,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>A$AP Ferg</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -8052,7 +8016,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Dua Lipa</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -8109,7 +8073,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>['numbers', '2021', 'rap', 'grime', 'alternative rap']</t>
+          <t>['2021', 'numbers', 'rap', 'grime', 'alternative rap']</t>
         </is>
       </c>
     </row>
@@ -8180,7 +8144,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t xml:space="preserve">Griselda </t>
+          <t>Griselda</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -8190,7 +8154,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -8210,11 +8174,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A244" t="inlineStr"/>
       <c r="B244" t="inlineStr">
         <is>
           <t>Cozy Tapes: Vol. 1 Friends-</t>
@@ -8274,11 +8234,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A246" t="inlineStr"/>
       <c r="B246" t="inlineStr">
         <is>
           <t>If It Bleeds, It Can Be Killed</t>
@@ -8286,7 +8242,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -8333,7 +8289,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>['jazz fusion', 'soul', '2020', 'funk', 'jazz']</t>
+          <t>['jazz fusion', 'soul', 'funk', 'jazz', 'neo-soul']</t>
         </is>
       </c>
     </row>
@@ -8350,7 +8306,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -8382,7 +8338,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -8429,7 +8385,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>['jazz rap', 'southern hip hop', 'rap', 'hip-hop', 'rick ross']</t>
+          <t>['rick ross', 'rap', 'hip-hop', '2017', 'jazz rap']</t>
         </is>
       </c>
     </row>
@@ -8446,7 +8402,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -8461,7 +8417,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', 'trap', '2 chainz', 'drake']</t>
+          <t>['rap', 'hip-hop', '2 chainz', 'trap', 'drake']</t>
         </is>
       </c>
     </row>
@@ -8493,7 +8449,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>['electronic', 'jazz', '2014', 'experimental', 'hip-hop']</t>
+          <t>['electronic', 'jazz', 'hip-hop', 'experimental', '2014']</t>
         </is>
       </c>
     </row>
@@ -8510,7 +8466,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -8606,7 +8562,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -8638,7 +8594,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -8653,7 +8609,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>['hip-hop', 'hip hop', 'rap', 'experimental hip hop', 'neo-psychedelia']</t>
+          <t>['hip-hop', 'hip hop', 'rap', '2018', 'experimental hip hop']</t>
         </is>
       </c>
     </row>
@@ -8670,7 +8626,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -8734,7 +8690,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -8761,27 +8717,27 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Dear Donda</t>
+          <t xml:space="preserve">Dear Donda </t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>5 tracks, 23:01</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>9 May 2021</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>['hip-hop', 'kanye west', 'rap', 'hip hop', 'soul']</t>
+          <t>['hip-hop', 'rap', 'hip hop', 'kanye west', 'rnb']</t>
         </is>
       </c>
     </row>
@@ -8798,7 +8754,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -8813,7 +8769,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>['neo-psychedelia', 'rap', 'hip-hop', 'neo soul', 'cloud rap']</t>
+          <t>['rap', 'neo-psychedelia', 'hip-hop', 'neo soul', 'cloud rap']</t>
         </is>
       </c>
     </row>
@@ -8894,12 +8850,12 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>24 tracks, 65:07</t>
+          <t>24 tracks, 64:50</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -8958,7 +8914,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -8990,7 +8946,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -9005,7 +8961,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>['2016', 'rnb', 'soul', 'hip hop', 'funk']</t>
+          <t>['funk', 'neo-soul', 'soul', 'psychedelic soul', 'rnb']</t>
         </is>
       </c>
     </row>
@@ -9293,7 +9249,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>['rap', 'hip-hop', 'sampling', 'rhythmic', 'boom bap']</t>
+          <t>['sampling', 'rhythmic', 'gangsta rap', 'male vocals', 'boom bap']</t>
         </is>
       </c>
     </row>
@@ -9357,7 +9313,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>['drake', 'rnb', 'hip hop', 'rap', 'trap']</t>
+          <t>['drake', 'hip hop', 'trap', 'rap', 'rnb']</t>
         </is>
       </c>
     </row>
@@ -9524,7 +9480,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>MÃ¥neskin</t>
+          <t>MÃƒÂ¥neskin</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -9549,7 +9505,7 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>['tok1d', 'rock', '4', 'ai', '7 out of 10']</t>
+          <t>['rock', 'tok1d', 'cover', 'kirshchecore', 'funky']</t>
         </is>
       </c>
     </row>
@@ -9603,7 +9559,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>15 tracks</t>
+          <t>15 tracks, 49:51</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9645,14 +9601,14 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>['amine', 'hyperpop', '2021', 'rap', 'pop rap']</t>
+          <t>['rap', 'pop rap', 'juke', 'digicore', 'trap']</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Kanye West</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -9667,7 +9623,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>32 tracks</t>
+          <t>32 tracks, 129:40</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9997,7 +9953,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>['jazz fusion', '2017', 'funk', 'neo-soul', 'soul']</t>
+          <t>['jazz fusion', 'funk', 'soul', '2015', 'kendrick lamar']</t>
         </is>
       </c>
     </row>
@@ -10098,11 +10054,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A303" t="inlineStr"/>
       <c r="B303" t="inlineStr">
         <is>
           <t>DAWN FM</t>
@@ -10196,7 +10148,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Cream</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -10418,11 +10370,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A313" t="inlineStr"/>
       <c r="B313" t="inlineStr">
         <is>
           <t>COWBOY BEBOP Soundtrack</t>
@@ -10477,7 +10425,7 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>['romantic', 'indie', 'joaoaksnes', 'soft rock', 'alt-country']</t>
+          <t>['digital tendencies', 'wsum 91.7 fm madison', 'indie', 'joaoaksnes', 'soft rock']</t>
         </is>
       </c>
     </row>
@@ -10772,7 +10720,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Lil Wayne</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -10893,7 +10841,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>['rnb', 'soul', 'electronic', 'hip hop', 'alternative rnb']</t>
+          <t>['rnb', 'soul', 'electronic', 'alternative rnb', 'hip hop']</t>
         </is>
       </c>
     </row>
@@ -10996,7 +10944,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Error fetch</t>
+          <t>Nanku</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -11284,7 +11232,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>The Smiths</t>
+          <t>Error fetch</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -11341,7 +11289,7 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>['slowcore', 'shoegaze', 'depressive', 'alternative rock', 'indie rock']</t>
+          <t>['shoegaze', 'slowcore', 'indie rock', 'song name describes me', 'rock']</t>
         </is>
       </c>
     </row>
@@ -11363,7 +11311,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>8 tracks, 40:11</t>
+          <t>8 tracks, 41:21</t>
         </is>
       </c>
       <c r="E342" t="inlineStr">
@@ -11506,11 +11454,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr">
-        <is>
-          <t>Error fetch</t>
-        </is>
-      </c>
+      <c r="A347" t="inlineStr"/>
       <c r="B347" t="inlineStr">
         <is>
           <t>King of the Mischievous South Vol. 2</t>
@@ -11597,7 +11541,7 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>['kanye west', '2021', 'rap', 'hip hop', 'yzy snd']</t>
+          <t>['2021', 'kanye west', 'rap', 'hip hop', 'yzy snd']</t>
         </is>
       </c>
     </row>
@@ -11779,7 +11723,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>3 tracks, 16:23</t>
+          <t>3 tracks, 17:22</t>
         </is>
       </c>
       <c r="E355" t="inlineStr">
@@ -12003,7 +11947,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>11 tracks, 50:21</t>
+          <t>11 tracks, 49:29</t>
         </is>
       </c>
       <c r="E362" t="inlineStr">
@@ -12014,6 +11958,70 @@
       <c r="F362" t="inlineStr">
         <is>
           <t>['soul', 'pop', 'female vocalists', 'adele', 'british']</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Clairo</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Immunity</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>11 tracks, 40:36</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>2 August 2019</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>['bedroom pop', '2019', 'dream pop', 'indie pop', 'indietronica']</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Last.fm</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Rammstein</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>1994 – present (31 years)</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>Berlin, Germany</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>['industrial metal', 'metal', 'industrial', 'german', 'rock']</t>
         </is>
       </c>
     </row>

</xml_diff>